<commit_message>
el inicio la prueba con regresion lineal de datos de puntos equipo y partidos ganados y en especial EL MODELO ELO de incio ya funciona en parte falta la parte web e integrar la base de datos
</commit_message>
<xml_diff>
--- a/Datos/2020-Apertura.xlsx
+++ b/Datos/2020-Apertura.xlsx
@@ -542,7 +542,7 @@
         <v>46</v>
       </c>
       <c r="J5">
-        <v>1500</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="6">
@@ -712,7 +712,7 @@
         <v>38</v>
       </c>
       <c r="J10">
-        <v>1500</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="11">

</xml_diff>